<commit_message>
Introduced POIJI for mapping the sheet with Java Class.
Updated the ExcelReaderReaderUtil2.java to map the sheet with java
class.

Uses Generics for making the code reusable!
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/PhoenixTestData.xlsx
+++ b/src/test/resources/testData/PhoenixTestData.xlsx
@@ -244,7 +244,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -266,18 +266,18 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created the DataProvider Util for the excel data that is used in the Createjob api test
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/PhoenixTestData.xlsx
+++ b/src/test/resources/testData/PhoenixTestData.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="CreateJobTestData" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="56">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -35,6 +36,159 @@
   </si>
   <si>
     <t xml:space="preserve">iamsup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mst_service_location_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mst_platform_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mst_warrenty_status_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mst_oem_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer__first_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer__last_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer__mobile_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer__mobile_number_alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer__email_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer__email_id_alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_address__flat_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_address__apartment_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_address__street_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_address__landmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_address__area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_address__pincode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_address__country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_address__state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_product__dop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_product__serial_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_product__imei1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_product__imei2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_product__popurl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_product__product_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_product__mst_model_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">problems__id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">problems__remark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halvorson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">308-982-2512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layne.Turcotte@yahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c 304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jupiter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MG road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangur Nagar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goregaon West</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maharashtra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-06T18:30:00.000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56391087191268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery Issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jatin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56391087191342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajinkya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56391087191235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56391087194567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ritu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56391034591268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kajal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56391456191268</t>
   </si>
 </sst>
 </file>
@@ -44,7 +198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -66,6 +220,13 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -84,7 +245,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -108,8 +269,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -118,14 +283,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal 2" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -243,7 +413,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -290,4 +460,613 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AA7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA4" activeCellId="0" sqref="AA4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="25.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="24.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="22.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="23.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="25.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="28.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="16.04"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>411039</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>411039</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>411039</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>411039</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>411039</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>411039</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>